<commit_message>
Update market data and stock prices
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/dumps/Stocks/Oil India Ltd.xlsx
+++ b/dumps/Stocks/Oil India Ltd.xlsx
@@ -751,7 +751,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP970"/>
+  <dimension ref="A1:AP972"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="5">
       <c r="A5" s="87" t="n">
-        <v>46049</v>
+        <v>45954</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1114,21 +1114,18 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
-        <v>440.35</v>
+        <v>424.1</v>
       </c>
       <c r="F5" t="n">
-        <v>2212.75</v>
+        <v>8482</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>CN#252611030591</t>
+          <t>~</t>
         </is>
-      </c>
-      <c r="I5" t="n">
-        <v>11</v>
       </c>
       <c r="J5">
         <f>Index!$C$2</f>
@@ -1137,7 +1134,7 @@
     </row>
     <row r="6">
       <c r="A6" s="87" t="n">
-        <v>45996</v>
+        <v>45953</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
@@ -1150,21 +1147,18 @@
         </is>
       </c>
       <c r="D6" s="0" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>409.3</v>
+        <v>420</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>2056.75</v>
+        <v>8400</v>
       </c>
       <c r="G6" s="0" t="inlineStr">
         <is>
-          <t>CN#252609039305</t>
+          <t>~</t>
         </is>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>10.25</v>
       </c>
       <c r="J6" s="0">
         <f>Index!$C$2</f>
@@ -1173,7 +1167,7 @@
     </row>
     <row r="7">
       <c r="A7" s="87" t="n">
-        <v>45957</v>
+        <v>46049</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
@@ -1186,226 +1180,102 @@
         </is>
       </c>
       <c r="D7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>440.35</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>2212.75</v>
+      </c>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t>CN#252611030591</t>
+        </is>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="J7" s="0">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="87" t="n">
+        <v>45996</v>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>409.3</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2056.75</v>
+      </c>
+      <c r="G8" s="0" t="inlineStr">
+        <is>
+          <t>CN#252609039305</t>
+        </is>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>10.25</v>
+      </c>
+      <c r="J8" s="0">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="87" t="n">
+        <v>45957</v>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C9" s="0" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D9" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E9" s="0" t="n">
         <v>421.25</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <v>4233.6</v>
       </c>
-      <c r="G7" s="0" t="inlineStr">
+      <c r="G9" s="0" t="inlineStr">
         <is>
           <t>CN#252607382790</t>
         </is>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I9" s="0" t="n">
         <v>21.1</v>
       </c>
-      <c r="J7" s="0">
+      <c r="J9" s="0">
         <f>Index!$C$2</f>
         <v/>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="38" t="n">
-        <v>45950</v>
-      </c>
-      <c r="B8" s="39" t="inlineStr">
-        <is>
-          <t>NSE</t>
-        </is>
-      </c>
-      <c r="C8" s="39" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
-      <c r="D8" s="40" t="n">
-        <v>20</v>
-      </c>
-      <c r="E8" s="41" t="n">
-        <v>410.49</v>
-      </c>
-      <c r="F8" s="41">
-        <f>(D5*E5)</f>
-        <v/>
-      </c>
-      <c r="G8" s="39" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
-      <c r="H8" s="40" t="n"/>
-      <c r="I8" s="40" t="n"/>
-      <c r="J8" s="42">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K8" s="43">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), L5/sum(F5:I5), "")</f>
-        <v/>
-      </c>
-      <c r="L8" s="44">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
-        <v/>
-      </c>
-      <c r="M8" s="44">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), ((E5*D5)+L5), "")</f>
-        <v/>
-      </c>
-      <c r="N8" s="45">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), D5, "")</f>
-        <v/>
-      </c>
-      <c r="O8" s="43">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365), P5/sum(F5:I5), "")</f>
-        <v/>
-      </c>
-      <c r="P8" s="44">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
-        <v/>
-      </c>
-      <c r="Q8" s="44">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365), ((E5*D5)+P5), "")</f>
-        <v/>
-      </c>
-      <c r="R8" s="44">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365), D5, "")</f>
-        <v/>
-      </c>
-      <c r="S8" s="46">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365), T5/sum(F5:I5), "")</f>
-        <v/>
-      </c>
-      <c r="T8" s="47">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
-        <v/>
-      </c>
-      <c r="U8" s="47">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365), ((E5*D5)+T5), "")</f>
-        <v/>
-      </c>
-      <c r="V8" s="47">
-        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365), D5, "")</f>
-        <v/>
-      </c>
-      <c r="W8" s="47" t="n"/>
-      <c r="X8" s="47" t="n"/>
-      <c r="Y8" s="46">
-        <f>IF(AND( C5="Buy", W5&lt;&gt;"", AA5&lt;&gt;"", B5&lt;&gt;"DIV"), Z5/sum(F5:I5), "")</f>
-        <v/>
-      </c>
-      <c r="Z8" s="47" t="n"/>
-      <c r="AA8" s="47" t="n"/>
-      <c r="AB8" s="48" t="n"/>
-      <c r="AC8" s="44">
-        <f>if(B5="DIV", F5,"")</f>
-        <v/>
-      </c>
-      <c r="AD8" s="49" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="38" t="n">
-        <v>45947</v>
-      </c>
-      <c r="B9" s="39" t="inlineStr">
-        <is>
-          <t>NSE</t>
-        </is>
-      </c>
-      <c r="C9" s="39" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
-      <c r="D9" s="40" t="n">
-        <v>10</v>
-      </c>
-      <c r="E9" s="41" t="n">
-        <v>413.61</v>
-      </c>
-      <c r="F9" s="41">
-        <f>(D6*E6)+I6</f>
-        <v/>
-      </c>
-      <c r="G9" s="39" t="inlineStr">
-        <is>
-          <t>~</t>
-        </is>
-      </c>
-      <c r="H9" s="40" t="n"/>
-      <c r="I9" s="40" t="n"/>
-      <c r="J9" s="42">
-        <f>Index!$C$2</f>
-        <v/>
-      </c>
-      <c r="K9" s="43">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), L6/sum(F6:I6), "")</f>
-        <v/>
-      </c>
-      <c r="L9" s="44">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
-        <v/>
-      </c>
-      <c r="M9" s="44">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), ((E6*D6)+L6), "")</f>
-        <v/>
-      </c>
-      <c r="N9" s="45">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), D6, "")</f>
-        <v/>
-      </c>
-      <c r="O9" s="43">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365), P6/sum(F6:I6), "")</f>
-        <v/>
-      </c>
-      <c r="P9" s="44">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
-        <v/>
-      </c>
-      <c r="Q9" s="44">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365), ((E6*D6)+P6), "")</f>
-        <v/>
-      </c>
-      <c r="R9" s="44">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365), D6, "")</f>
-        <v/>
-      </c>
-      <c r="S9" s="46">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365), T6/sum(F6:I6), "")</f>
-        <v/>
-      </c>
-      <c r="T9" s="47">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
-        <v/>
-      </c>
-      <c r="U9" s="47">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365), ((E6*D6)+T6), "")</f>
-        <v/>
-      </c>
-      <c r="V9" s="47">
-        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365), D6, "")</f>
-        <v/>
-      </c>
-      <c r="W9" s="47" t="n"/>
-      <c r="X9" s="47" t="n"/>
-      <c r="Y9" s="46">
-        <f>IF(AND( C6="Buy", W6&lt;&gt;"", AA6&lt;&gt;"", B6&lt;&gt;"DIV"), Z6/sum(F6:I6), "")</f>
-        <v/>
-      </c>
-      <c r="Z9" s="47" t="n"/>
-      <c r="AA9" s="47" t="n"/>
-      <c r="AB9" s="48" t="n"/>
-      <c r="AC9" s="44">
-        <f>if(B6="DIV", F6,"")</f>
-        <v/>
-      </c>
-      <c r="AD9" s="49" t="n"/>
-    </row>
     <row r="10">
       <c r="A10" s="38" t="n">
-        <v>45924</v>
+        <v>45950</v>
       </c>
       <c r="B10" s="39" t="inlineStr">
         <is>
@@ -1421,10 +1291,10 @@
         <v>20</v>
       </c>
       <c r="E10" s="41" t="n">
-        <v>407.88</v>
+        <v>410.49</v>
       </c>
       <c r="F10" s="41">
-        <f>(D7*E7)+I7</f>
+        <f>(D5*E5)</f>
         <v/>
       </c>
       <c r="G10" s="39" t="inlineStr">
@@ -1439,75 +1309,75 @@
         <v/>
       </c>
       <c r="K10" s="43">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/sum(F7:I7), "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), L5/sum(F5:I5), "")</f>
         <v/>
       </c>
       <c r="L10" s="44">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
         <v/>
       </c>
       <c r="M10" s="44">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), ((E5*D5)+L5), "")</f>
         <v/>
       </c>
       <c r="N10" s="45">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV"), D5, "")</f>
         <v/>
       </c>
       <c r="O10" s="43">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/sum(F7:I7), "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365), P5/sum(F5:I5), "")</f>
         <v/>
       </c>
       <c r="P10" s="44">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
         <v/>
       </c>
       <c r="Q10" s="44">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365), ((E5*D5)+P5), "")</f>
         <v/>
       </c>
       <c r="R10" s="44">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &lt; 365), D5, "")</f>
         <v/>
       </c>
       <c r="S10" s="46">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/sum(F7:I7), "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365), T5/sum(F5:I5), "")</f>
         <v/>
       </c>
       <c r="T10" s="47">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365), (1-Index!$F$2*2)*((J5*D5)-(E5*D5)), "")</f>
         <v/>
       </c>
       <c r="U10" s="47">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365), ((E5*D5)+T5), "")</f>
         <v/>
       </c>
       <c r="V10" s="47">
-        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
+        <f>IF(AND( C5="Buy", ISBLANK(W5), B5&lt;&gt;"DIV", NOW()-A5 &gt; 365), D5, "")</f>
         <v/>
       </c>
       <c r="W10" s="47" t="n"/>
       <c r="X10" s="47" t="n"/>
       <c r="Y10" s="46">
-        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/sum(F7:I7), "")</f>
+        <f>IF(AND( C5="Buy", W5&lt;&gt;"", AA5&lt;&gt;"", B5&lt;&gt;"DIV"), Z5/sum(F5:I5), "")</f>
         <v/>
       </c>
       <c r="Z10" s="47" t="n"/>
       <c r="AA10" s="47" t="n"/>
       <c r="AB10" s="48" t="n"/>
       <c r="AC10" s="44">
-        <f>if(B7="DIV", F7,"")</f>
+        <f>if(B5="DIV", F5,"")</f>
         <v/>
       </c>
       <c r="AD10" s="49" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="38" t="n">
-        <v>45904</v>
+        <v>45947</v>
       </c>
       <c r="B11" s="39" t="inlineStr">
         <is>
-          <t>DIV</t>
+          <t>NSE</t>
         </is>
       </c>
       <c r="C11" s="39" t="inlineStr">
@@ -1516,95 +1386,92 @@
         </is>
       </c>
       <c r="D11" s="40" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E11" s="41" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F11" s="41" t="n">
-        <v>75</v>
+        <v>413.61</v>
+      </c>
+      <c r="F11" s="41">
+        <f>(D6*E6)+I6</f>
+        <v/>
       </c>
       <c r="G11" s="39" t="inlineStr">
         <is>
-          <t>Final-Dividend of Rs.1.5000/- per share on Ex-Date: 04-SEP-2025</t>
+          <t>~</t>
         </is>
       </c>
-      <c r="H11" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="40" t="n">
-        <v>0</v>
-      </c>
+      <c r="H11" s="40" t="n"/>
+      <c r="I11" s="40" t="n"/>
       <c r="J11" s="42">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K11" s="43">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/sum(F8:I8), "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), L6/sum(F6:I6), "")</f>
         <v/>
       </c>
       <c r="L11" s="44">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
         <v/>
       </c>
       <c r="M11" s="44">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), ((E6*D6)+L6), "")</f>
         <v/>
       </c>
       <c r="N11" s="45">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV"), D6, "")</f>
         <v/>
       </c>
       <c r="O11" s="43">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/sum(F8:I8), "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365), P6/sum(F6:I6), "")</f>
         <v/>
       </c>
       <c r="P11" s="44">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
         <v/>
       </c>
       <c r="Q11" s="44">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365), ((E6*D6)+P6), "")</f>
         <v/>
       </c>
       <c r="R11" s="44">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &lt; 365), D6, "")</f>
         <v/>
       </c>
       <c r="S11" s="46">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/sum(F8:I8), "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365), T6/sum(F6:I6), "")</f>
         <v/>
       </c>
       <c r="T11" s="47">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365), (1-Index!$F$2*2)*((J6*D6)-(E6*D6)), "")</f>
         <v/>
       </c>
       <c r="U11" s="47">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365), ((E6*D6)+T6), "")</f>
         <v/>
       </c>
       <c r="V11" s="47">
-        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
+        <f>IF(AND( C6="Buy", ISBLANK(W6), B6&lt;&gt;"DIV", NOW()-A6 &gt; 365), D6, "")</f>
         <v/>
       </c>
       <c r="W11" s="47" t="n"/>
       <c r="X11" s="47" t="n"/>
       <c r="Y11" s="46">
-        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/sum(F8:I8), "")</f>
+        <f>IF(AND( C6="Buy", W6&lt;&gt;"", AA6&lt;&gt;"", B6&lt;&gt;"DIV"), Z6/sum(F6:I6), "")</f>
         <v/>
       </c>
       <c r="Z11" s="47" t="n"/>
       <c r="AA11" s="47" t="n"/>
       <c r="AB11" s="48" t="n"/>
       <c r="AC11" s="44">
-        <f>if(B8="DIV", F8,"")</f>
+        <f>if(B6="DIV", F6,"")</f>
         <v/>
       </c>
       <c r="AD11" s="49" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="38" t="n">
-        <v>45855</v>
+        <v>45924</v>
       </c>
       <c r="B12" s="39" t="inlineStr">
         <is>
@@ -1620,96 +1487,93 @@
         <v>20</v>
       </c>
       <c r="E12" s="41" t="n">
-        <v>451.08</v>
-      </c>
-      <c r="F12" s="41" t="n">
-        <v>9021.52</v>
+        <v>407.88</v>
+      </c>
+      <c r="F12" s="41">
+        <f>(D7*E7)+I7</f>
+        <v/>
       </c>
       <c r="G12" s="39" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H12" s="40" t="n">
-        <v>8.960000000000001</v>
-      </c>
-      <c r="I12" s="40" t="n">
-        <v>54.56</v>
-      </c>
+      <c r="H12" s="40" t="n"/>
+      <c r="I12" s="40" t="n"/>
       <c r="J12" s="42">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K12" s="43">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/sum(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), L7/sum(F7:I7), "")</f>
         <v/>
       </c>
       <c r="L12" s="44">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="M12" s="44">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), ((E7*D7)+L7), "")</f>
         <v/>
       </c>
       <c r="N12" s="45">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV"), D7, "")</f>
         <v/>
       </c>
       <c r="O12" s="43">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/sum(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), P7/sum(F7:I7), "")</f>
         <v/>
       </c>
       <c r="P12" s="44">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="Q12" s="44">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), ((E7*D7)+P7), "")</f>
         <v/>
       </c>
       <c r="R12" s="44">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &lt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="S12" s="46">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/sum(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), T7/sum(F7:I7), "")</f>
         <v/>
       </c>
       <c r="T12" s="47">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), (1-Index!$F$2*2)*((J7*D7)-(E7*D7)), "")</f>
         <v/>
       </c>
       <c r="U12" s="47">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), ((E7*D7)+T7), "")</f>
         <v/>
       </c>
       <c r="V12" s="47">
-        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
+        <f>IF(AND( C7="Buy", ISBLANK(W7), B7&lt;&gt;"DIV", NOW()-A7 &gt; 365), D7, "")</f>
         <v/>
       </c>
       <c r="W12" s="47" t="n"/>
       <c r="X12" s="47" t="n"/>
       <c r="Y12" s="46">
-        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/sum(F9:I9), "")</f>
+        <f>IF(AND( C7="Buy", W7&lt;&gt;"", AA7&lt;&gt;"", B7&lt;&gt;"DIV"), Z7/sum(F7:I7), "")</f>
         <v/>
       </c>
       <c r="Z12" s="47" t="n"/>
       <c r="AA12" s="47" t="n"/>
       <c r="AB12" s="48" t="n"/>
       <c r="AC12" s="44">
-        <f>if(B9="DIV", F9,"")</f>
+        <f>if(B7="DIV", F7,"")</f>
         <v/>
       </c>
       <c r="AD12" s="49" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="38" t="n">
-        <v>45811</v>
+        <v>45904</v>
       </c>
       <c r="B13" s="39" t="inlineStr">
         <is>
-          <t>NSE</t>
+          <t>DIV</t>
         </is>
       </c>
       <c r="C13" s="39" t="inlineStr">
@@ -1718,95 +1582,95 @@
         </is>
       </c>
       <c r="D13" s="40" t="n">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E13" s="41" t="n">
-        <v>425.19</v>
+        <v>1.5</v>
       </c>
       <c r="F13" s="41" t="n">
-        <v>1275.57</v>
+        <v>75</v>
       </c>
       <c r="G13" s="39" t="inlineStr">
         <is>
-          <t>~</t>
+          <t>Final-Dividend of Rs.1.5000/- per share on Ex-Date: 04-SEP-2025</t>
         </is>
       </c>
       <c r="H13" s="40" t="n">
-        <v>1.27</v>
+        <v>0</v>
       </c>
       <c r="I13" s="40" t="n">
-        <v>7.7</v>
+        <v>0</v>
       </c>
       <c r="J13" s="42">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K13" s="43">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), L10/sum(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), L8/sum(F8:I8), "")</f>
         <v/>
       </c>
       <c r="L13" s="44">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="M13" s="44">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), ((E10*D10)+L10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), ((E8*D8)+L8), "")</f>
         <v/>
       </c>
       <c r="N13" s="45">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), D10, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV"), D8, "")</f>
         <v/>
       </c>
       <c r="O13" s="43">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), P10/sum(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), P8/sum(F8:I8), "")</f>
         <v/>
       </c>
       <c r="P13" s="44">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="Q13" s="44">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), ((E10*D10)+P10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), ((E8*D8)+P8), "")</f>
         <v/>
       </c>
       <c r="R13" s="44">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), D10, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &lt; 365), D8, "")</f>
         <v/>
       </c>
       <c r="S13" s="46">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), T10/sum(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), T8/sum(F8:I8), "")</f>
         <v/>
       </c>
       <c r="T13" s="47">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), (1-Index!$F$2*2)*((J8*D8)-(E8*D8)), "")</f>
         <v/>
       </c>
       <c r="U13" s="47">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), ((E10*D10)+T10), "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), ((E8*D8)+T8), "")</f>
         <v/>
       </c>
       <c r="V13" s="47">
-        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), D10, "")</f>
+        <f>IF(AND( C8="Buy", ISBLANK(W8), B8&lt;&gt;"DIV", NOW()-A8 &gt; 365), D8, "")</f>
         <v/>
       </c>
       <c r="W13" s="47" t="n"/>
       <c r="X13" s="47" t="n"/>
       <c r="Y13" s="46">
-        <f>IF(AND( C10="Buy", W10&lt;&gt;"", AA10&lt;&gt;"", B10&lt;&gt;"DIV"), Z10/sum(F10:I10), "")</f>
+        <f>IF(AND( C8="Buy", W8&lt;&gt;"", AA8&lt;&gt;"", B8&lt;&gt;"DIV"), Z8/sum(F8:I8), "")</f>
         <v/>
       </c>
       <c r="Z13" s="47" t="n"/>
       <c r="AA13" s="47" t="n"/>
       <c r="AB13" s="48" t="n"/>
       <c r="AC13" s="44">
-        <f>if(B10="DIV", F10,"")</f>
+        <f>if(B8="DIV", F8,"")</f>
         <v/>
       </c>
       <c r="AD13" s="49" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="38" t="n">
-        <v>45811</v>
+        <v>45855</v>
       </c>
       <c r="B14" s="39" t="inlineStr">
         <is>
@@ -1819,13 +1683,13 @@
         </is>
       </c>
       <c r="D14" s="40" t="n">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E14" s="41" t="n">
-        <v>425.19</v>
+        <v>451.08</v>
       </c>
       <c r="F14" s="41" t="n">
-        <v>850.38</v>
+        <v>9021.52</v>
       </c>
       <c r="G14" s="39" t="inlineStr">
         <is>
@@ -1833,74 +1697,74 @@
         </is>
       </c>
       <c r="H14" s="40" t="n">
-        <v>0.84</v>
+        <v>8.960000000000001</v>
       </c>
       <c r="I14" s="40" t="n">
-        <v>5.14</v>
+        <v>54.56</v>
       </c>
       <c r="J14" s="42">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K14" s="43">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), L11/sum(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), L9/sum(F9:I9), "")</f>
         <v/>
       </c>
       <c r="L14" s="44">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="M14" s="44">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), ((E11*D11)+L11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), ((E9*D9)+L9), "")</f>
         <v/>
       </c>
       <c r="N14" s="45">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), D11, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV"), D9, "")</f>
         <v/>
       </c>
       <c r="O14" s="43">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), P11/sum(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), P9/sum(F9:I9), "")</f>
         <v/>
       </c>
       <c r="P14" s="44">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="Q14" s="44">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), ((E11*D11)+P11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), ((E9*D9)+P9), "")</f>
         <v/>
       </c>
       <c r="R14" s="44">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), D11, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &lt; 365), D9, "")</f>
         <v/>
       </c>
       <c r="S14" s="46">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), T11/sum(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), T9/sum(F9:I9), "")</f>
         <v/>
       </c>
       <c r="T14" s="47">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), (1-Index!$F$2*2)*((J9*D9)-(E9*D9)), "")</f>
         <v/>
       </c>
       <c r="U14" s="47">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), ((E11*D11)+T11), "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), ((E9*D9)+T9), "")</f>
         <v/>
       </c>
       <c r="V14" s="47">
-        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), D11, "")</f>
+        <f>IF(AND( C9="Buy", ISBLANK(W9), B9&lt;&gt;"DIV", NOW()-A9 &gt; 365), D9, "")</f>
         <v/>
       </c>
       <c r="W14" s="47" t="n"/>
       <c r="X14" s="47" t="n"/>
       <c r="Y14" s="46">
-        <f>IF(AND( C11="Buy", W11&lt;&gt;"", AA11&lt;&gt;"", B11&lt;&gt;"DIV"), Z11/sum(F11:I11), "")</f>
+        <f>IF(AND( C9="Buy", W9&lt;&gt;"", AA9&lt;&gt;"", B9&lt;&gt;"DIV"), Z9/sum(F9:I9), "")</f>
         <v/>
       </c>
       <c r="Z14" s="47" t="n"/>
       <c r="AA14" s="47" t="n"/>
       <c r="AB14" s="48" t="n"/>
       <c r="AC14" s="44">
-        <f>if(B11="DIV", F11,"")</f>
+        <f>if(B9="DIV", F9,"")</f>
         <v/>
       </c>
       <c r="AD14" s="49" t="n"/>
@@ -1920,13 +1784,13 @@
         </is>
       </c>
       <c r="D15" s="40" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15" s="41" t="n">
         <v>425.19</v>
       </c>
       <c r="F15" s="41" t="n">
-        <v>2125.97</v>
+        <v>1275.57</v>
       </c>
       <c r="G15" s="39" t="inlineStr">
         <is>
@@ -1934,311 +1798,481 @@
         </is>
       </c>
       <c r="H15" s="40" t="n">
-        <v>2.11</v>
+        <v>1.27</v>
       </c>
       <c r="I15" s="40" t="n">
-        <v>12.86</v>
+        <v>7.7</v>
       </c>
       <c r="J15" s="42">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K15" s="43">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), L12/sum(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), L10/sum(F10:I10), "")</f>
         <v/>
       </c>
       <c r="L15" s="44">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="M15" s="44">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), ((E12*D12)+L12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), ((E10*D10)+L10), "")</f>
         <v/>
       </c>
       <c r="N15" s="45">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), D12, "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV"), D10, "")</f>
         <v/>
       </c>
       <c r="O15" s="43">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), P12/sum(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), P10/sum(F10:I10), "")</f>
         <v/>
       </c>
       <c r="P15" s="44">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="Q15" s="44">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), ((E12*D12)+P12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), ((E10*D10)+P10), "")</f>
         <v/>
       </c>
       <c r="R15" s="44">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), D12, "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &lt; 365), D10, "")</f>
         <v/>
       </c>
       <c r="S15" s="46">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), T12/sum(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), T10/sum(F10:I10), "")</f>
         <v/>
       </c>
       <c r="T15" s="47">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), (1-Index!$F$2*2)*((J10*D10)-(E10*D10)), "")</f>
         <v/>
       </c>
       <c r="U15" s="47">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), ((E12*D12)+T12), "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), ((E10*D10)+T10), "")</f>
         <v/>
       </c>
       <c r="V15" s="47">
-        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), D12, "")</f>
+        <f>IF(AND( C10="Buy", ISBLANK(W10), B10&lt;&gt;"DIV", NOW()-A10 &gt; 365), D10, "")</f>
         <v/>
       </c>
       <c r="W15" s="47" t="n"/>
       <c r="X15" s="47" t="n"/>
       <c r="Y15" s="46">
-        <f>IF(AND( C12="Buy", W12&lt;&gt;"", AA12&lt;&gt;"", B12&lt;&gt;"DIV"), Z12/sum(F12:I12), "")</f>
+        <f>IF(AND( C10="Buy", W10&lt;&gt;"", AA10&lt;&gt;"", B10&lt;&gt;"DIV"), Z10/sum(F10:I10), "")</f>
         <v/>
       </c>
       <c r="Z15" s="47" t="n"/>
       <c r="AA15" s="47" t="n"/>
       <c r="AB15" s="48" t="n"/>
       <c r="AC15" s="44">
-        <f>if(B12="DIV", F12,"")</f>
+        <f>if(B10="DIV", F10,"")</f>
         <v/>
       </c>
       <c r="AD15" s="49" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="50" t="n">
-        <v>45705</v>
-      </c>
-      <c r="B16" s="51" t="inlineStr">
+      <c r="A16" s="38" t="n">
+        <v>45811</v>
+      </c>
+      <c r="B16" s="39" t="inlineStr">
         <is>
           <t>NSE</t>
         </is>
       </c>
-      <c r="C16" s="51" t="inlineStr">
+      <c r="C16" s="39" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
       </c>
-      <c r="D16" s="52" t="n">
-        <v>12</v>
-      </c>
-      <c r="E16" s="53" t="n">
-        <v>383.85</v>
-      </c>
-      <c r="F16" s="53" t="n">
-        <v>4606.24</v>
-      </c>
-      <c r="G16" s="51" t="inlineStr">
+      <c r="D16" s="40" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="41" t="n">
+        <v>425.19</v>
+      </c>
+      <c r="F16" s="41" t="n">
+        <v>850.38</v>
+      </c>
+      <c r="G16" s="39" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H16" s="52" t="n">
-        <v>4.56</v>
-      </c>
-      <c r="I16" s="52" t="n">
-        <v>27.88</v>
+      <c r="H16" s="40" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="I16" s="40" t="n">
+        <v>5.14</v>
       </c>
       <c r="J16" s="42">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K16" s="43">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/sum(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), L11/sum(F11:I11), "")</f>
         <v/>
       </c>
       <c r="L16" s="44">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="M16" s="44">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), ((E11*D11)+L11), "")</f>
         <v/>
       </c>
       <c r="N16" s="45">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV"), D11, "")</f>
         <v/>
       </c>
       <c r="O16" s="43">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/sum(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), P11/sum(F11:I11), "")</f>
         <v/>
       </c>
       <c r="P16" s="44">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="Q16" s="44">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), ((E11*D11)+P11), "")</f>
         <v/>
       </c>
       <c r="R16" s="44">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &lt; 365), D11, "")</f>
         <v/>
       </c>
       <c r="S16" s="46">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/sum(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), T11/sum(F11:I11), "")</f>
         <v/>
       </c>
       <c r="T16" s="47">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), (1-Index!$F$2*2)*((J11*D11)-(E11*D11)), "")</f>
         <v/>
       </c>
       <c r="U16" s="47">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), ((E11*D11)+T11), "")</f>
         <v/>
       </c>
       <c r="V16" s="47">
-        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
+        <f>IF(AND( C11="Buy", ISBLANK(W11), B11&lt;&gt;"DIV", NOW()-A11 &gt; 365), D11, "")</f>
         <v/>
       </c>
       <c r="W16" s="47" t="n"/>
       <c r="X16" s="47" t="n"/>
       <c r="Y16" s="46">
-        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/sum(F13:I13), "")</f>
+        <f>IF(AND( C11="Buy", W11&lt;&gt;"", AA11&lt;&gt;"", B11&lt;&gt;"DIV"), Z11/sum(F11:I11), "")</f>
         <v/>
       </c>
       <c r="Z16" s="47" t="n"/>
       <c r="AA16" s="47" t="n"/>
       <c r="AB16" s="48" t="n"/>
       <c r="AC16" s="44">
-        <f>if(B13="DIV", F13,"")</f>
+        <f>if(B11="DIV", F11,"")</f>
         <v/>
       </c>
       <c r="AD16" s="49" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="50" t="n">
-        <v>45705</v>
-      </c>
-      <c r="B17" s="51" t="inlineStr">
+      <c r="A17" s="38" t="n">
+        <v>45811</v>
+      </c>
+      <c r="B17" s="39" t="inlineStr">
         <is>
           <t>NSE</t>
         </is>
       </c>
-      <c r="C17" s="51" t="inlineStr">
+      <c r="C17" s="39" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
       </c>
-      <c r="D17" s="52" t="n">
-        <v>8</v>
-      </c>
-      <c r="E17" s="53" t="n">
-        <v>383.91</v>
-      </c>
-      <c r="F17" s="53" t="n">
-        <v>3071.26</v>
-      </c>
-      <c r="G17" s="51" t="inlineStr">
+      <c r="D17" s="40" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" s="41" t="n">
+        <v>425.19</v>
+      </c>
+      <c r="F17" s="41" t="n">
+        <v>2125.97</v>
+      </c>
+      <c r="G17" s="39" t="inlineStr">
         <is>
           <t>~</t>
         </is>
       </c>
-      <c r="H17" s="52" t="n">
-        <v>3.05</v>
-      </c>
-      <c r="I17" s="52" t="n">
-        <v>18.61</v>
+      <c r="H17" s="40" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="I17" s="40" t="n">
+        <v>12.86</v>
       </c>
       <c r="J17" s="42">
         <f>Index!$C$2</f>
         <v/>
       </c>
       <c r="K17" s="43">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/sum(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), L12/sum(F12:I12), "")</f>
         <v/>
       </c>
       <c r="L17" s="44">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="M17" s="44">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), ((E12*D12)+L12), "")</f>
         <v/>
       </c>
       <c r="N17" s="45">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV"), D12, "")</f>
         <v/>
       </c>
       <c r="O17" s="43">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/sum(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), P12/sum(F12:I12), "")</f>
         <v/>
       </c>
       <c r="P17" s="44">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="Q17" s="44">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), ((E12*D12)+P12), "")</f>
         <v/>
       </c>
       <c r="R17" s="44">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &lt; 365), D12, "")</f>
         <v/>
       </c>
       <c r="S17" s="46">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/sum(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), T12/sum(F12:I12), "")</f>
         <v/>
       </c>
       <c r="T17" s="47">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), (1-Index!$F$2*2)*((J12*D12)-(E12*D12)), "")</f>
         <v/>
       </c>
       <c r="U17" s="47">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), ((E12*D12)+T12), "")</f>
         <v/>
       </c>
       <c r="V17" s="47">
-        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
+        <f>IF(AND( C12="Buy", ISBLANK(W12), B12&lt;&gt;"DIV", NOW()-A12 &gt; 365), D12, "")</f>
         <v/>
       </c>
       <c r="W17" s="47" t="n"/>
       <c r="X17" s="47" t="n"/>
       <c r="Y17" s="46">
-        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/sum(F14:I14), "")</f>
+        <f>IF(AND( C12="Buy", W12&lt;&gt;"", AA12&lt;&gt;"", B12&lt;&gt;"DIV"), Z12/sum(F12:I12), "")</f>
         <v/>
       </c>
       <c r="Z17" s="47" t="n"/>
       <c r="AA17" s="47" t="n"/>
       <c r="AB17" s="48" t="n"/>
       <c r="AC17" s="44">
+        <f>if(B12="DIV", F12,"")</f>
+        <v/>
+      </c>
+      <c r="AD17" s="49" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="50" t="n">
+        <v>45705</v>
+      </c>
+      <c r="B18" s="51" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C18" s="51" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D18" s="52" t="n">
+        <v>12</v>
+      </c>
+      <c r="E18" s="53" t="n">
+        <v>383.85</v>
+      </c>
+      <c r="F18" s="53" t="n">
+        <v>4606.24</v>
+      </c>
+      <c r="G18" s="51" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="H18" s="52" t="n">
+        <v>4.56</v>
+      </c>
+      <c r="I18" s="52" t="n">
+        <v>27.88</v>
+      </c>
+      <c r="J18" s="42">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K18" s="43">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), L13/sum(F13:I13), "")</f>
+        <v/>
+      </c>
+      <c r="L18" s="44">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <v/>
+      </c>
+      <c r="M18" s="44">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), ((E13*D13)+L13), "")</f>
+        <v/>
+      </c>
+      <c r="N18" s="45">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV"), D13, "")</f>
+        <v/>
+      </c>
+      <c r="O18" s="43">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), P13/sum(F13:I13), "")</f>
+        <v/>
+      </c>
+      <c r="P18" s="44">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <v/>
+      </c>
+      <c r="Q18" s="44">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), ((E13*D13)+P13), "")</f>
+        <v/>
+      </c>
+      <c r="R18" s="44">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &lt; 365), D13, "")</f>
+        <v/>
+      </c>
+      <c r="S18" s="46">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), T13/sum(F13:I13), "")</f>
+        <v/>
+      </c>
+      <c r="T18" s="47">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), (1-Index!$F$2*2)*((J13*D13)-(E13*D13)), "")</f>
+        <v/>
+      </c>
+      <c r="U18" s="47">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), ((E13*D13)+T13), "")</f>
+        <v/>
+      </c>
+      <c r="V18" s="47">
+        <f>IF(AND( C13="Buy", ISBLANK(W13), B13&lt;&gt;"DIV", NOW()-A13 &gt; 365), D13, "")</f>
+        <v/>
+      </c>
+      <c r="W18" s="47" t="n"/>
+      <c r="X18" s="47" t="n"/>
+      <c r="Y18" s="46">
+        <f>IF(AND( C13="Buy", W13&lt;&gt;"", AA13&lt;&gt;"", B13&lt;&gt;"DIV"), Z13/sum(F13:I13), "")</f>
+        <v/>
+      </c>
+      <c r="Z18" s="47" t="n"/>
+      <c r="AA18" s="47" t="n"/>
+      <c r="AB18" s="48" t="n"/>
+      <c r="AC18" s="44">
+        <f>if(B13="DIV", F13,"")</f>
+        <v/>
+      </c>
+      <c r="AD18" s="49" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="50" t="n">
+        <v>45705</v>
+      </c>
+      <c r="B19" s="51" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C19" s="51" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D19" s="52" t="n">
+        <v>8</v>
+      </c>
+      <c r="E19" s="53" t="n">
+        <v>383.91</v>
+      </c>
+      <c r="F19" s="53" t="n">
+        <v>3071.26</v>
+      </c>
+      <c r="G19" s="51" t="inlineStr">
+        <is>
+          <t>~</t>
+        </is>
+      </c>
+      <c r="H19" s="52" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="I19" s="52" t="n">
+        <v>18.61</v>
+      </c>
+      <c r="J19" s="42">
+        <f>Index!$C$2</f>
+        <v/>
+      </c>
+      <c r="K19" s="43">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), L14/sum(F14:I14), "")</f>
+        <v/>
+      </c>
+      <c r="L19" s="44">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <v/>
+      </c>
+      <c r="M19" s="44">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), ((E14*D14)+L14), "")</f>
+        <v/>
+      </c>
+      <c r="N19" s="45">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV"), D14, "")</f>
+        <v/>
+      </c>
+      <c r="O19" s="43">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), P14/sum(F14:I14), "")</f>
+        <v/>
+      </c>
+      <c r="P19" s="44">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <v/>
+      </c>
+      <c r="Q19" s="44">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), ((E14*D14)+P14), "")</f>
+        <v/>
+      </c>
+      <c r="R19" s="44">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &lt; 365), D14, "")</f>
+        <v/>
+      </c>
+      <c r="S19" s="46">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), T14/sum(F14:I14), "")</f>
+        <v/>
+      </c>
+      <c r="T19" s="47">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), (1-Index!$F$2*2)*((J14*D14)-(E14*D14)), "")</f>
+        <v/>
+      </c>
+      <c r="U19" s="47">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), ((E14*D14)+T14), "")</f>
+        <v/>
+      </c>
+      <c r="V19" s="47">
+        <f>IF(AND( C14="Buy", ISBLANK(W14), B14&lt;&gt;"DIV", NOW()-A14 &gt; 365), D14, "")</f>
+        <v/>
+      </c>
+      <c r="W19" s="47" t="n"/>
+      <c r="X19" s="47" t="n"/>
+      <c r="Y19" s="46">
+        <f>IF(AND( C14="Buy", W14&lt;&gt;"", AA14&lt;&gt;"", B14&lt;&gt;"DIV"), Z14/sum(F14:I14), "")</f>
+        <v/>
+      </c>
+      <c r="Z19" s="47" t="n"/>
+      <c r="AA19" s="47" t="n"/>
+      <c r="AB19" s="48" t="n"/>
+      <c r="AC19" s="44">
         <f>if(B14="DIV", F14,"")</f>
         <v/>
       </c>
-      <c r="AD17" s="49" t="n"/>
-    </row>
-    <row r="18">
-      <c r="E18" s="54" t="n"/>
-      <c r="F18" s="54" t="n"/>
-      <c r="G18" s="55" t="n"/>
-      <c r="J18" s="54" t="n"/>
-      <c r="K18" s="54" t="n"/>
-      <c r="L18" s="54" t="n"/>
-      <c r="M18" s="57" t="n"/>
-      <c r="W18" s="54" t="n"/>
-      <c r="X18" s="54" t="n"/>
-      <c r="Y18" s="54" t="n"/>
-      <c r="Z18" s="54" t="n"/>
-      <c r="AA18" s="54" t="n"/>
-      <c r="AB18" s="54" t="n"/>
-      <c r="AC18" s="54" t="n"/>
-    </row>
-    <row r="19">
-      <c r="E19" s="54" t="n"/>
-      <c r="F19" s="54" t="n"/>
-      <c r="G19" s="55" t="n"/>
-      <c r="J19" s="54" t="n"/>
-      <c r="K19" s="54" t="n"/>
-      <c r="L19" s="54" t="n"/>
-      <c r="M19" s="57" t="n"/>
-      <c r="W19" s="54" t="n"/>
-      <c r="X19" s="54" t="n"/>
-      <c r="Y19" s="54" t="n"/>
-      <c r="Z19" s="54" t="n"/>
-      <c r="AA19" s="54" t="n"/>
-      <c r="AB19" s="54" t="n"/>
-      <c r="AC19" s="54" t="n"/>
+      <c r="AD19" s="49" t="n"/>
     </row>
     <row r="20">
       <c r="E20" s="54" t="n"/>
@@ -17191,6 +17225,7 @@
       <c r="J954" s="54" t="n"/>
       <c r="K954" s="54" t="n"/>
       <c r="L954" s="54" t="n"/>
+      <c r="M954" s="57" t="n"/>
       <c r="W954" s="54" t="n"/>
       <c r="X954" s="54" t="n"/>
       <c r="Y954" s="54" t="n"/>
@@ -17206,6 +17241,7 @@
       <c r="J955" s="54" t="n"/>
       <c r="K955" s="54" t="n"/>
       <c r="L955" s="54" t="n"/>
+      <c r="M955" s="57" t="n"/>
       <c r="W955" s="54" t="n"/>
       <c r="X955" s="54" t="n"/>
       <c r="Y955" s="54" t="n"/>
@@ -17438,6 +17474,36 @@
       <c r="AA970" s="54" t="n"/>
       <c r="AB970" s="54" t="n"/>
       <c r="AC970" s="54" t="n"/>
+    </row>
+    <row r="971">
+      <c r="E971" s="54" t="n"/>
+      <c r="F971" s="54" t="n"/>
+      <c r="G971" s="55" t="n"/>
+      <c r="J971" s="54" t="n"/>
+      <c r="K971" s="54" t="n"/>
+      <c r="L971" s="54" t="n"/>
+      <c r="W971" s="54" t="n"/>
+      <c r="X971" s="54" t="n"/>
+      <c r="Y971" s="54" t="n"/>
+      <c r="Z971" s="54" t="n"/>
+      <c r="AA971" s="54" t="n"/>
+      <c r="AB971" s="54" t="n"/>
+      <c r="AC971" s="54" t="n"/>
+    </row>
+    <row r="972">
+      <c r="E972" s="54" t="n"/>
+      <c r="F972" s="54" t="n"/>
+      <c r="G972" s="55" t="n"/>
+      <c r="J972" s="54" t="n"/>
+      <c r="K972" s="54" t="n"/>
+      <c r="L972" s="54" t="n"/>
+      <c r="W972" s="54" t="n"/>
+      <c r="X972" s="54" t="n"/>
+      <c r="Y972" s="54" t="n"/>
+      <c r="Z972" s="54" t="n"/>
+      <c r="AA972" s="54" t="n"/>
+      <c r="AB972" s="54" t="n"/>
+      <c r="AC972" s="54" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="$A$4:$AO$44"/>

</xml_diff>